<commit_message>
add location check excel
</commit_message>
<xml_diff>
--- a/excel_data/002_Excel_Data_For_Practice(3).xlsx
+++ b/excel_data/002_Excel_Data_For_Practice(3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13ccd1b3724d3287/Articles/Excel Articles/Others/دیتابیس آماده اکسل برای تمرین/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amirhasan\Desktop\excel_convertor\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="11_F25DC773A252ABDACC10486DD15853105BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F81E63B8-973A-4393-8A8E-52CB9779FC31}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CAE581-B742-4E5B-990F-16655772F520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9013" uniqueCount="2051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9018" uniqueCount="2059">
   <si>
     <t>E02002</t>
   </si>
@@ -6178,6 +6178,30 @@
   </si>
   <si>
     <t>حقوق سالانه(دلار)</t>
+  </si>
+  <si>
+    <t>تهران</t>
+  </si>
+  <si>
+    <t>استان</t>
+  </si>
+  <si>
+    <t>پردیس</t>
+  </si>
+  <si>
+    <t>بومهن</t>
+  </si>
+  <si>
+    <t>مشهد</t>
+  </si>
+  <si>
+    <t>خانی آباد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اصفهان </t>
+  </si>
+  <si>
+    <t>آتشگاه</t>
   </si>
 </sst>
 </file>
@@ -6185,8 +6209,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -6223,14 +6247,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -6254,14 +6278,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>490347</xdr:colOff>
+      <xdr:colOff>128397</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>21075</xdr:rowOff>
     </xdr:to>
@@ -6306,13 +6330,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>381842</xdr:colOff>
+      <xdr:colOff>19892</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>43514</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>291164</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>21075</xdr:rowOff>
     </xdr:to>
@@ -6356,14 +6380,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>518922</xdr:colOff>
+      <xdr:colOff>156972</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>154425</xdr:rowOff>
     </xdr:to>
@@ -6407,14 +6431,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>149314</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>396964</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>169030</xdr:rowOff>
     </xdr:to>
@@ -6722,9 +6746,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1001"/>
+  <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6740,9 +6766,10 @@
     <col min="11" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2017</v>
       </c>
@@ -6782,8 +6809,11 @@
       <c r="M1" t="s">
         <v>2006</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6824,7 +6854,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6862,10 +6892,13 @@
         <v>1986</v>
       </c>
       <c r="M3" t="s">
-        <v>1991</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2055</v>
+      </c>
+      <c r="N3" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6906,7 +6939,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -6947,7 +6980,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -6985,10 +7018,13 @@
         <v>1986</v>
       </c>
       <c r="M6" t="s">
-        <v>1994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2051</v>
+      </c>
+      <c r="N6" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -7029,7 +7065,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -7067,10 +7103,13 @@
         <v>1987</v>
       </c>
       <c r="M8" t="s">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2051</v>
+      </c>
+      <c r="N8" t="s">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -7111,7 +7150,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -7152,7 +7191,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -7193,7 +7232,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -7234,7 +7273,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -7275,7 +7314,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -7313,10 +7352,13 @@
         <v>1987</v>
       </c>
       <c r="M14" t="s">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2057</v>
+      </c>
+      <c r="N14" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -7357,7 +7399,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>

</xml_diff>